<commit_message>
fix: response Login and form add data warga
</commit_message>
<xml_diff>
--- a/revisi_dataset_clean.xlsx
+++ b/revisi_dataset_clean.xlsx
@@ -845,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD72"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,11 +862,11 @@
     <col min="7" max="7" width="11" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>128</v>
       </c>
@@ -898,7 +898,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1571011507470060</v>
       </c>
@@ -929,9 +929,14 @@
       <c r="J2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1571011111840160</v>
       </c>
@@ -962,9 +967,14 @@
       <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1571010708580000</v>
       </c>
@@ -995,9 +1005,14 @@
       <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="3"/>
+      <c r="O4"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>1571010104790060</v>
       </c>
@@ -1028,9 +1043,14 @@
       <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K5" s="4"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5" s="3"/>
+      <c r="O5"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>1571011608840180</v>
       </c>
@@ -1061,9 +1081,14 @@
       <c r="J6" s="3">
         <v>2</v>
       </c>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K6" s="4"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>1571010909780100</v>
       </c>
@@ -1094,9 +1119,14 @@
       <c r="J7" s="3">
         <v>2</v>
       </c>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K7" s="4"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>1571012703750000</v>
       </c>
@@ -1127,9 +1157,14 @@
       <c r="J8" s="3">
         <v>2</v>
       </c>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K8" s="4"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>1571102512720000</v>
       </c>
@@ -1160,9 +1195,14 @@
       <c r="J9" s="3">
         <v>0</v>
       </c>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K9" s="4"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>1571011010540000</v>
       </c>
@@ -1193,9 +1233,14 @@
       <c r="J10" s="3">
         <v>0</v>
       </c>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>1571012802670020</v>
       </c>
@@ -1226,9 +1271,14 @@
       <c r="J11" s="3">
         <v>3</v>
       </c>
-      <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K11" s="4"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>1571014107820000</v>
       </c>
@@ -1259,9 +1309,14 @@
       <c r="J12" s="3">
         <v>0</v>
       </c>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>1571085004940060</v>
       </c>
@@ -1292,9 +1347,14 @@
       <c r="J13" s="3">
         <v>2</v>
       </c>
-      <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>1571010804810120</v>
       </c>
@@ -1325,9 +1385,14 @@
       <c r="J14" s="3">
         <v>1</v>
       </c>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>1505031304880000</v>
       </c>
@@ -1358,9 +1423,14 @@
       <c r="J15" s="3">
         <v>2</v>
       </c>
-      <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>1571082908870040</v>
       </c>
@@ -1391,9 +1461,14 @@
       <c r="J16" s="3">
         <v>2</v>
       </c>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>1571012006720060</v>
       </c>
@@ -1424,9 +1499,14 @@
       <c r="J17" s="3">
         <v>1</v>
       </c>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>1571010705690060</v>
       </c>
@@ -1457,9 +1537,14 @@
       <c r="J18" s="3">
         <v>3</v>
       </c>
-      <c r="L18" s="12"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>1571015212780060</v>
       </c>
@@ -1490,9 +1575,14 @@
       <c r="J19" s="3">
         <v>2</v>
       </c>
-      <c r="L19" s="12"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>1571011905570000</v>
       </c>
@@ -1523,9 +1613,14 @@
       <c r="J20" s="3">
         <v>0</v>
       </c>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>1571014406580000</v>
       </c>
@@ -1556,9 +1651,14 @@
       <c r="J21" s="3">
         <v>1</v>
       </c>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>1571014107690000</v>
       </c>
@@ -1589,9 +1689,14 @@
       <c r="J22" s="3">
         <v>3</v>
       </c>
-      <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>1571010606670000</v>
       </c>
@@ -1622,9 +1727,14 @@
       <c r="J23" s="3">
         <v>1</v>
       </c>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>1571010708800020</v>
       </c>
@@ -1655,9 +1765,14 @@
       <c r="J24" s="3">
         <v>1</v>
       </c>
-      <c r="L24" s="8"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>1571010608840020</v>
       </c>
@@ -1688,9 +1803,14 @@
       <c r="J25" s="3">
         <v>1</v>
       </c>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>1571014810910080</v>
       </c>
@@ -1721,9 +1841,14 @@
       <c r="J26" s="3">
         <v>3</v>
       </c>
-      <c r="L26" s="12"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>1571011903420020</v>
       </c>
@@ -1754,9 +1879,14 @@
       <c r="J27" s="3">
         <v>1</v>
       </c>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>1571012706670000</v>
       </c>
@@ -1787,9 +1917,14 @@
       <c r="J28" s="3">
         <v>1</v>
       </c>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>1571015601840060</v>
       </c>
@@ -1820,9 +1955,14 @@
       <c r="J29" s="3">
         <v>2</v>
       </c>
-      <c r="L29" s="12"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>1571070512880000</v>
       </c>
@@ -1853,9 +1993,14 @@
       <c r="J30" s="3">
         <v>1</v>
       </c>
-      <c r="L30" s="8"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>1571011509760020</v>
       </c>
@@ -1886,9 +2031,14 @@
       <c r="J31" s="3">
         <v>1</v>
       </c>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>1571015512790080</v>
       </c>
@@ -1919,9 +2069,14 @@
       <c r="J32" s="3">
         <v>2</v>
       </c>
-      <c r="L32" s="12"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>1571015702770000</v>
       </c>
@@ -1952,9 +2107,14 @@
       <c r="J33" s="3">
         <v>3</v>
       </c>
-      <c r="L33" s="12"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>1571011805770000</v>
       </c>
@@ -1985,9 +2145,14 @@
       <c r="J34" s="3">
         <v>0</v>
       </c>
-      <c r="L34" s="8"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>1571017112330180</v>
       </c>
@@ -2018,9 +2183,14 @@
       <c r="J35" s="3">
         <v>1</v>
       </c>
-      <c r="L35" s="8"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>1571011502470000</v>
       </c>
@@ -2051,9 +2221,14 @@
       <c r="J36" s="3">
         <v>0</v>
       </c>
-      <c r="L36" s="8"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>1571030207960020</v>
       </c>
@@ -2084,9 +2259,14 @@
       <c r="J37" s="3">
         <v>0</v>
       </c>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>1571015110950040</v>
       </c>
@@ -2117,9 +2297,14 @@
       <c r="J38" s="3">
         <v>0</v>
       </c>
-      <c r="L38" s="8"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
         <v>1571015202840020</v>
       </c>
@@ -2150,9 +2335,14 @@
       <c r="J39" s="3">
         <v>2</v>
       </c>
-      <c r="L39" s="12"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>1571011812860020</v>
       </c>
@@ -2183,9 +2373,14 @@
       <c r="J40" s="3">
         <v>0</v>
       </c>
-      <c r="L40" s="8"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="12">
         <v>1571016906820020</v>
       </c>
@@ -2216,9 +2411,14 @@
       <c r="J41" s="3">
         <v>2</v>
       </c>
-      <c r="L41" s="12"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>1571012411690020</v>
       </c>
@@ -2249,9 +2449,14 @@
       <c r="J42" s="3">
         <v>1</v>
       </c>
-      <c r="L42" s="8"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>1505071403920000</v>
       </c>
@@ -2282,9 +2487,14 @@
       <c r="J43" s="3">
         <v>1</v>
       </c>
-      <c r="L43" s="8"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <v>1571015608670020</v>
       </c>
@@ -2315,9 +2525,14 @@
       <c r="J44" s="3">
         <v>0</v>
       </c>
-      <c r="L44" s="8"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>1571015005520080</v>
       </c>
@@ -2348,9 +2563,14 @@
       <c r="J45" s="3">
         <v>0</v>
       </c>
-      <c r="L45" s="8"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="12">
         <v>1571015107880100</v>
       </c>
@@ -2381,9 +2601,14 @@
       <c r="J46" s="3">
         <v>3</v>
       </c>
-      <c r="L46" s="12"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>1571014210780040</v>
       </c>
@@ -2414,9 +2639,14 @@
       <c r="J47" s="3">
         <v>2</v>
       </c>
-      <c r="L47" s="12"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <v>1571011202930000</v>
       </c>
@@ -2447,9 +2677,14 @@
       <c r="J48" s="3">
         <v>1</v>
       </c>
-      <c r="L48" s="8"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="12">
         <v>1571076006820200</v>
       </c>
@@ -2480,9 +2715,14 @@
       <c r="J49" s="3">
         <v>2</v>
       </c>
-      <c r="L49" s="12"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>1571012006730080</v>
       </c>
@@ -2513,9 +2753,14 @@
       <c r="J50" s="3">
         <v>1</v>
       </c>
-      <c r="L50" s="8"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>1571011010570120</v>
       </c>
@@ -2546,9 +2791,14 @@
       <c r="J51" s="3">
         <v>0</v>
       </c>
-      <c r="L51" s="8"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>1571015011590000</v>
       </c>
@@ -2579,9 +2829,14 @@
       <c r="J52" s="3">
         <v>0</v>
       </c>
-      <c r="L52" s="8"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>1571075512690040</v>
       </c>
@@ -2612,9 +2867,14 @@
       <c r="J53" s="3">
         <v>0</v>
       </c>
-      <c r="L53" s="8"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="O53"/>
+      <c r="P53"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>1511021010790000</v>
       </c>
@@ -2645,9 +2905,14 @@
       <c r="J54" s="3">
         <v>1</v>
       </c>
-      <c r="L54" s="8"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+      <c r="P54"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="12">
         <v>1571014101810320</v>
       </c>
@@ -2678,9 +2943,14 @@
       <c r="J55" s="3">
         <v>1</v>
       </c>
-      <c r="L55" s="12"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="12">
         <v>1571014901710000</v>
       </c>
@@ -2711,9 +2981,14 @@
       <c r="J56" s="3">
         <v>1</v>
       </c>
-      <c r="L56" s="12"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="O56"/>
+      <c r="P56"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="12">
         <v>1571015612640000</v>
       </c>
@@ -2744,9 +3019,14 @@
       <c r="J57" s="3">
         <v>1</v>
       </c>
-      <c r="L57" s="12"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57"/>
+      <c r="P57"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>1571012807870020</v>
       </c>
@@ -2777,9 +3057,14 @@
       <c r="J58" s="3">
         <v>2</v>
       </c>
-      <c r="L58" s="8"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="O58"/>
+      <c r="P58"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>1571011303810040</v>
       </c>
@@ -2810,9 +3095,14 @@
       <c r="J59" s="3">
         <v>0</v>
       </c>
-      <c r="L59" s="8"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59"/>
+      <c r="P59"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>1571010711330000</v>
       </c>
@@ -2843,9 +3133,14 @@
       <c r="J60" s="3">
         <v>0</v>
       </c>
-      <c r="L60" s="8"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60"/>
+      <c r="P60"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>1571014506610040</v>
       </c>
@@ -2876,9 +3171,14 @@
       <c r="J61" s="3">
         <v>2</v>
       </c>
-      <c r="L61" s="8"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="O61"/>
+      <c r="P61"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>1571012812500000</v>
       </c>
@@ -2909,9 +3209,14 @@
       <c r="J62" s="3">
         <v>0</v>
       </c>
-      <c r="L62" s="8"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="N62"/>
+      <c r="O62"/>
+      <c r="P62"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="12">
         <v>1571015702690000</v>
       </c>
@@ -2942,9 +3247,14 @@
       <c r="J63" s="3">
         <v>3</v>
       </c>
-      <c r="L63" s="12"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+      <c r="N63"/>
+      <c r="O63"/>
+      <c r="P63"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>1606054101880000</v>
       </c>
@@ -2975,9 +3285,14 @@
       <c r="J64" s="3">
         <v>0</v>
       </c>
-      <c r="L64" s="8"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+      <c r="N64"/>
+      <c r="O64"/>
+      <c r="P64"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
         <v>1571014502660060</v>
       </c>
@@ -3008,9 +3323,14 @@
       <c r="J65" s="3">
         <v>2</v>
       </c>
-      <c r="L65" s="8"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="O65"/>
+      <c r="P65"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
         <v>1571021204690060</v>
       </c>
@@ -3041,9 +3361,14 @@
       <c r="J66" s="3">
         <v>2</v>
       </c>
-      <c r="L66" s="8"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
         <v>1571014508680020</v>
       </c>
@@ -3074,9 +3399,14 @@
       <c r="J67" s="3">
         <v>0</v>
       </c>
-      <c r="L67" s="8"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="8">
         <v>1571014303670000</v>
       </c>
@@ -3107,9 +3437,14 @@
       <c r="J68" s="3">
         <v>0</v>
       </c>
-      <c r="L68" s="8"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K68"/>
+      <c r="L68"/>
+      <c r="M68"/>
+      <c r="N68"/>
+      <c r="O68"/>
+      <c r="P68"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="12">
         <v>1571014409840000</v>
       </c>
@@ -3140,9 +3475,14 @@
       <c r="J69" s="3">
         <v>3</v>
       </c>
-      <c r="L69" s="12"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K69"/>
+      <c r="L69"/>
+      <c r="M69"/>
+      <c r="N69"/>
+      <c r="O69"/>
+      <c r="P69"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="12">
         <v>1571012210800080</v>
       </c>
@@ -3173,9 +3513,14 @@
       <c r="J70" s="3">
         <v>3</v>
       </c>
-      <c r="L70" s="12"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K70"/>
+      <c r="L70"/>
+      <c r="M70"/>
+      <c r="N70"/>
+      <c r="O70"/>
+      <c r="P70"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="12">
         <v>1571016302860040</v>
       </c>
@@ -3206,9 +3551,14 @@
       <c r="J71" s="3">
         <v>3</v>
       </c>
-      <c r="L71" s="12"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+      <c r="N71"/>
+      <c r="O71"/>
+      <c r="P71"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="8">
         <v>1571016512700000</v>
       </c>
@@ -3239,7 +3589,12 @@
       <c r="J72" s="3">
         <v>2</v>
       </c>
-      <c r="L72" s="8"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72"/>
+      <c r="O72"/>
+      <c r="P72"/>
     </row>
   </sheetData>
   <sortState ref="A2:L72">

</xml_diff>